<commit_message>
removed CB R23 due to Git LFS quota limit (Doh!)
</commit_message>
<xml_diff>
--- a/Rankings.xlsx
+++ b/Rankings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\BrsVgl\Performance Efficiency Suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\BrsVgl\PerformanceEfficiencySuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2F98DB-DDDA-4908-8861-06A8B21D4E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742B216-7335-4487-8BB1-BE53E5EA3D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="8" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>CPU</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Poekel</t>
   </si>
   <si>
-    <t>Ryzen 7 4750G (Renoir)</t>
-  </si>
-  <si>
     <t>Summe von PES MT</t>
   </si>
   <si>
@@ -124,9 +122,6 @@
     <t>dosenfisch24</t>
   </si>
   <si>
-    <t>AMD Ryzen 7 4750U</t>
-  </si>
-  <si>
     <t>Sweepi</t>
   </si>
   <si>
@@ -136,22 +131,46 @@
     <t>AMD Ryzen 5 3600 (Matisse) [2]</t>
   </si>
   <si>
-    <t>AMD Razyen 7 3700X (Matisse) [5]</t>
-  </si>
-  <si>
-    <t>??? [7]</t>
-  </si>
-  <si>
     <t>Intel i7 1065G (IceLake) [3]</t>
   </si>
   <si>
     <t>AMD Ryzen 7 4700U (Renoir) [1]</t>
   </si>
   <si>
-    <t>AMD Ryzen 7 4750U [6]</t>
+    <t>AMD Razyen 9 5950X (Vermeer)</t>
   </si>
   <si>
-    <t>Ryzen 7 4750G (Renoir) [4]</t>
+    <t>AMD Razyen 7 3700X (Matisse) [6]</t>
+  </si>
+  <si>
+    <t>??? [8]</t>
+  </si>
+  <si>
+    <t>AMD Razyen 9 5950X (Vermeer) [4]</t>
+  </si>
+  <si>
+    <t>Duration ST</t>
+  </si>
+  <si>
+    <t>Average Power ST</t>
+  </si>
+  <si>
+    <t>Duration MT</t>
+  </si>
+  <si>
+    <t>Average Power MT</t>
+  </si>
+  <si>
+    <t>AMDRyzen 7 4750G (Renoir)</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 4750U (Renoir)</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7 4750U (Renoir) [7]</t>
+  </si>
+  <si>
+    <t>AMDRyzen 7 4750G (Renoir) [5]</t>
   </si>
 </sst>
 </file>
@@ -609,39 +628,42 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PES ST'!$B$3:$B$10</c:f>
+              <c:f>'PES ST'!$B$3:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>AMD Razyen 7 3700X (Matisse) [5]</c:v>
+                  <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>??? [7]</c:v>
+                  <c:v>??? [8]</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>AMD Ryzen 7 4750U [6]</c:v>
+                <c:pt idx="6">
+                  <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>Ryzen 7 4750G (Renoir) [4]</c:v>
+                <c:pt idx="7">
+                  <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PES ST'!$C$3:$C$10</c:f>
+              <c:f>'PES ST'!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>45.76</c:v>
                 </c:pt>
@@ -652,15 +674,18 @@
                   <c:v>52.94</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>55.41</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>127.76</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>133.62</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>137.88</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>153.88</c:v>
                 </c:pt>
               </c:numCache>
@@ -713,7 +738,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1357,28 +1382,31 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Consumption ST'!$B$3:$B$10</c:f>
+              <c:f>'Consumption ST'!$B$3:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>??? [7]</c:v>
+                  <c:v>??? [8]</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>AMD Razyen 7 3700X (Matisse) [5]</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>AMD Ryzen 7 4750U [6]</c:v>
+                  <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Ryzen 7 4750G (Renoir) [4]</c:v>
+                  <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
               </c:strCache>
@@ -1386,29 +1414,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Consumption ST'!$C$3:$C$10</c:f>
+              <c:f>'Consumption ST'!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>37274</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>35920</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>32112</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30057</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10396</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>10352</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10168</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>9839</c:v>
                 </c:pt>
               </c:numCache>
@@ -1461,7 +1492,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2105,9 +2136,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PES MT'!$B$3:$B$10</c:f>
+              <c:f>'PES MT'!$B$3:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
@@ -2115,29 +2146,32 @@
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>AMD Razyen 7 3700X (Matisse) [5]</c:v>
+                  <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Ryzen 7 4750G (Renoir) [4]</c:v>
+                  <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>AMD Ryzen 7 4750U [6]</c:v>
+                  <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>??? [7]</c:v>
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>??? [8]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PES MT'!$C$3:$C$10</c:f>
+              <c:f>'PES MT'!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>885.22</c:v>
                 </c:pt>
@@ -2157,6 +2191,9 @@
                   <c:v>3599.63</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>4779.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5760.71</c:v>
                 </c:pt>
               </c:numCache>
@@ -2209,7 +2246,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2882,6 +2919,62 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -2972,39 +3065,42 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Consumption MT'!$B$3:$B$10</c:f>
+              <c:f>'Consumption MT'!$B$3:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>AMD Razyen 7 3700X (Matisse) [5]</c:v>
+                  <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Ryzen 7 4750G (Renoir) [4]</c:v>
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>??? [7]</c:v>
+                  <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>??? [8]</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>AMD Ryzen 7 4750U [6]</c:v>
+                <c:pt idx="7">
+                  <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Consumption MT'!$C$3:$C$10</c:f>
+              <c:f>'Consumption MT'!$C$3:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>7223</c:v>
                 </c:pt>
@@ -3012,18 +3108,21 @@
                   <c:v>6377</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6242</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5262</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4507</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>3912</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2649</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2029</c:v>
                 </c:pt>
               </c:numCache>
@@ -3031,7 +3130,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-81B1-44D1-A529-DE37BAD97AFF}"/>
+              <c16:uniqueId val="{00000001-38A4-49BE-B1FD-5A7803352B11}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3076,7 +3175,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5397,14 +5496,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5446,8 +5545,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5489,8 +5588,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5532,8 +5631,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5564,37 +5663,98 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44370.941889814814" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="7" xr:uid="{1C48AB18-201F-498F-BA2B-FB5C4F62805E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44370.982344444441" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{1C48AB18-201F-498F-BA2B-FB5C4F62805E}">
   <cacheSource type="worksheet">
-    <worksheetSource name="GeneralTable[[GraphLabel]:[Consumption MT]]"/>
+    <worksheetSource name="GeneralTable[[GraphLabel]:[PES MT]]"/>
   </cacheSource>
-  <cacheFields count="5">
+  <cacheFields count="6">
     <cacheField name="GraphLabel" numFmtId="0">
-      <sharedItems count="11">
+      <sharedItems count="18">
         <s v="AMD Ryzen 7 4700U (Renoir) [1]"/>
         <s v="AMD Ryzen 5 3600 (Matisse) [2]"/>
         <s v="Intel i7 1065G (IceLake) [3]"/>
-        <s v="Ryzen 7 4750G (Renoir) [4]"/>
-        <s v="AMD Razyen 7 3700X (Matisse) [5]"/>
-        <s v="AMD Ryzen 7 4750U [6]"/>
-        <s v="??? [7]"/>
+        <s v="AMD Razyen 9 5950X (Vermeer) [4]"/>
+        <s v="AMDRyzen 7 4750G (Renoir) [5]"/>
+        <s v="AMD Razyen 7 3700X (Matisse) [6]"/>
+        <s v="AMD Ryzen 7 4750U (Renoir) [7]"/>
+        <s v="??? [8]"/>
         <s v="Ryzen 7 4750G (Renoir) [18]" u="1"/>
+        <s v="AMD Ryzen 7 4750U [6]" u="1"/>
+        <s v="Intel i7 1065G (IceLake) [7]" u="1"/>
+        <s v="AMD Ryzen 5 3600 (Matisse) [6]" u="1"/>
+        <s v="AMD Ryzen 7 4750U [7]" u="1"/>
+        <s v="??? [7]" u="1"/>
+        <s v="Ryzen 7 4750G (Renoir) [4]" u="1"/>
+        <s v="Ryzen 7 4750G (Renoir) [5]" u="1"/>
+        <s v="AMD Razyen 7 3700X (Matisse) [5]" u="1"/>
         <s v="AMD Ryzen 7 4700U (Renoir) [3]" u="1"/>
-        <s v="AMD Ryzen 5 3600 (Matisse) [6]" u="1"/>
-        <s v="Intel i7 1065G (IceLake) [7]" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="PES ST" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.76" maxValue="153.88"/>
     </cacheField>
+    <cacheField name="Consumption ST" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9839" maxValue="37274"/>
+    </cacheField>
+    <cacheField name="Duration ST" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="502.43" maxValue="502.43"/>
+    </cacheField>
+    <cacheField name="Average Power ST" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="71.489999999999995" maxValue="71.489999999999995"/>
+    </cacheField>
     <cacheField name="PES MT" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="885.22" maxValue="5760.71"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44370.984763657405" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{77F125F5-FAEA-41C0-B4FE-830A225910E6}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="GeneralTable[[GraphLabel]:[Average Power MT]]"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="GraphLabel" numFmtId="0">
+      <sharedItems count="8">
+        <s v="AMD Ryzen 7 4700U (Renoir) [1]"/>
+        <s v="AMD Ryzen 5 3600 (Matisse) [2]"/>
+        <s v="Intel i7 1065G (IceLake) [3]"/>
+        <s v="AMD Razyen 9 5950X (Vermeer) [4]"/>
+        <s v="AMDRyzen 7 4750G (Renoir) [5]"/>
+        <s v="AMD Razyen 7 3700X (Matisse) [6]"/>
+        <s v="AMD Ryzen 7 4750U (Renoir) [7]"/>
+        <s v="??? [8]"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="PES ST" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.76" maxValue="153.88"/>
     </cacheField>
     <cacheField name="Consumption ST" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9839" maxValue="37274"/>
     </cacheField>
+    <cacheField name="Duration ST" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="502.43" maxValue="502.43"/>
+    </cacheField>
+    <cacheField name="Average Power ST" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="71.489999999999995" maxValue="71.489999999999995"/>
+    </cacheField>
+    <cacheField name="PES MT" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="885.22" maxValue="5760.71"/>
+    </cacheField>
     <cacheField name="Consumption MT" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2029" maxValue="7223"/>
+    </cacheField>
+    <cacheField name="Duration MT" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="33.520000000000003" maxValue="33.520000000000003"/>
+    </cacheField>
+    <cacheField name="Average Power MT" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="186.22" maxValue="186.22"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -5606,75 +5766,190 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="7">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
   <r>
     <x v="0"/>
     <n v="133.62"/>
+    <n v="10168"/>
+    <m/>
+    <m/>
     <n v="2586.7600000000002"/>
-    <n v="10168"/>
-    <n v="2649"/>
   </r>
   <r>
     <x v="1"/>
     <n v="45.76"/>
+    <n v="32112"/>
+    <m/>
+    <m/>
     <n v="1386.39"/>
-    <n v="32112"/>
-    <n v="7223"/>
   </r>
   <r>
     <x v="2"/>
     <n v="127.76"/>
+    <n v="9839"/>
+    <m/>
+    <m/>
     <n v="885.22"/>
-    <n v="9839"/>
-    <n v="3912"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="153.88"/>
-    <n v="2637.56"/>
-    <n v="10352"/>
-    <n v="5262"/>
+    <n v="55.41"/>
+    <n v="35920"/>
+    <n v="502.43"/>
+    <n v="71.489999999999995"/>
+    <n v="4779.3"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="51.8"/>
-    <n v="2058.48"/>
-    <n v="30057"/>
-    <n v="6377"/>
+    <n v="153.88"/>
+    <n v="10352"/>
+    <m/>
+    <m/>
+    <n v="2637.56"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="137.88"/>
-    <n v="3599.63"/>
-    <n v="10396"/>
-    <n v="2029"/>
+    <n v="51.8"/>
+    <n v="30057"/>
+    <m/>
+    <m/>
+    <n v="2058.48"/>
   </r>
   <r>
     <x v="6"/>
+    <n v="137.88"/>
+    <n v="10396"/>
+    <m/>
+    <m/>
+    <n v="3599.63"/>
+  </r>
+  <r>
+    <x v="7"/>
     <n v="52.94"/>
+    <n v="37274"/>
+    <m/>
+    <m/>
     <n v="5760.71"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+  <r>
+    <x v="0"/>
+    <n v="133.62"/>
+    <n v="10168"/>
+    <m/>
+    <m/>
+    <n v="2586.7600000000002"/>
+    <n v="2649"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="45.76"/>
+    <n v="32112"/>
+    <m/>
+    <m/>
+    <n v="1386.39"/>
+    <n v="7223"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="127.76"/>
+    <n v="9839"/>
+    <m/>
+    <m/>
+    <n v="885.22"/>
+    <n v="3912"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="55.41"/>
+    <n v="35920"/>
+    <n v="502.43"/>
+    <n v="71.489999999999995"/>
+    <n v="4779.3"/>
+    <n v="6242"/>
+    <n v="33.520000000000003"/>
+    <n v="186.22"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="153.88"/>
+    <n v="10352"/>
+    <m/>
+    <m/>
+    <n v="2637.56"/>
+    <n v="5262"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="51.8"/>
+    <n v="30057"/>
+    <m/>
+    <m/>
+    <n v="2058.48"/>
+    <n v="6377"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="137.88"/>
+    <n v="10396"/>
+    <m/>
+    <m/>
+    <n v="3599.63"/>
+    <n v="2029"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="52.94"/>
     <n v="37274"/>
+    <m/>
+    <m/>
+    <n v="5760.71"/>
     <n v="4507"/>
+    <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53C9821C-4AAD-4B7A-89BF-B6F792D64CD3}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="B2:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53C9821C-4AAD-4B7A-89BF-B6F792D64CD3}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="12">
-        <item m="1" x="9"/>
+      <items count="19">
+        <item m="1" x="11"/>
+        <item m="1" x="17"/>
+        <item m="1" x="10"/>
         <item m="1" x="8"/>
-        <item m="1" x="10"/>
-        <item m="1" x="7"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="14"/>
+        <item m="1" x="16"/>
+        <item m="1" x="9"/>
+        <item m="1" x="13"/>
         <item x="3"/>
+        <item m="1" x="15"/>
+        <item x="5"/>
+        <item m="1" x="12"/>
+        <item x="7"/>
         <item x="4"/>
-        <item x="5"/>
         <item x="6"/>
         <item t="default"/>
       </items>
@@ -5692,19 +5967,23 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x v="5"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="13"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="11"/>
     </i>
     <i>
       <x v="6"/>
@@ -5713,10 +5992,10 @@
       <x v="4"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="17"/>
     </i>
     <i>
-      <x v="7"/>
+      <x v="16"/>
     </i>
     <i t="grand">
       <x/>
@@ -5752,21 +6031,28 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42BB440A-B501-4946-B14C-754D93D31B67}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="B2:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42BB440A-B501-4946-B14C-754D93D31B67}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="12">
-        <item m="1" x="9"/>
+      <items count="19">
+        <item m="1" x="11"/>
+        <item m="1" x="17"/>
+        <item m="1" x="10"/>
         <item m="1" x="8"/>
-        <item m="1" x="10"/>
-        <item m="1" x="7"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="14"/>
+        <item m="1" x="16"/>
+        <item m="1" x="9"/>
+        <item m="1" x="13"/>
         <item x="3"/>
+        <item m="1" x="15"/>
+        <item x="5"/>
+        <item m="1" x="12"/>
+        <item x="7"/>
         <item x="4"/>
-        <item x="5"/>
         <item x="6"/>
         <item t="default"/>
       </items>
@@ -5781,28 +6067,32 @@
       </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
-      <x v="10"/>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="11"/>
     </i>
     <i>
       <x v="5"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="13"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="17"/>
     </i>
     <i>
-      <x v="7"/>
+      <x v="16"/>
     </i>
     <i>
       <x v="4"/>
@@ -5818,7 +6108,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Summe von Consumption ST" fld="3" baseField="0" baseItem="0" numFmtId="3"/>
+    <dataField name="Summe von Consumption ST" fld="2" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="3" format="5" series="1">
@@ -5844,21 +6134,28 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BEB41E7C-5AB2-4580-B381-A37610DCF2EB}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="B2:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BEB41E7C-5AB2-4580-B381-A37610DCF2EB}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="12">
-        <item m="1" x="9"/>
+      <items count="19">
+        <item m="1" x="11"/>
+        <item m="1" x="17"/>
+        <item m="1" x="10"/>
         <item m="1" x="8"/>
-        <item m="1" x="10"/>
-        <item m="1" x="7"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="14"/>
+        <item m="1" x="16"/>
+        <item m="1" x="9"/>
+        <item m="1" x="13"/>
         <item x="3"/>
+        <item m="1" x="15"/>
+        <item x="5"/>
+        <item m="1" x="12"/>
+        <item x="7"/>
         <item x="4"/>
-        <item x="5"/>
         <item x="6"/>
         <item t="default"/>
       </items>
@@ -5873,14 +6170,15 @@
       </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x v="6"/>
     </i>
@@ -5888,19 +6186,22 @@
       <x v="5"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="13"/>
     </i>
     <i>
       <x v="4"/>
     </i>
     <i>
-      <x v="7"/>
+      <x v="16"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="17"/>
     </i>
     <i>
-      <x v="10"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="15"/>
     </i>
     <i t="grand">
       <x/>
@@ -5910,7 +6211,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Summe von PES MT" fld="2" baseField="0" baseItem="1" numFmtId="4"/>
+    <dataField name="Summe von PES MT" fld="5" baseField="0" baseItem="1" numFmtId="4"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="3" format="5" series="1">
@@ -5936,21 +6237,18 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0E6F04D-ED3A-40EC-8D2F-503A358EE722}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="B2:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2EE254DA-8EFF-4861-8DBF-B2F3ACC4A6C4}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="12">
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item m="1" x="10"/>
-        <item m="1" x="7"/>
+      <items count="9">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
+        <item x="5"/>
+        <item x="7"/>
         <item x="4"/>
-        <item x="5"/>
         <item x="6"/>
         <item t="default"/>
       </items>
@@ -5967,32 +6265,39 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
-      <x v="5"/>
+      <x v="1"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="10"/>
+      <x v="3"/>
     </i>
     <i>
       <x v="6"/>
     </i>
     <i>
-      <x v="4"/>
+      <x v="5"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -6002,28 +6307,10 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Summe von Consumption MT" fld="4" baseField="0" baseItem="1" numFmtId="4"/>
+    <dataField name="Summe von Consumption MT" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="4" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="9" series="1">
+  <chartFormats count="1">
+    <chartFormat chart="4" format="8" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -6046,9 +6333,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}" name="GeneralTable" displayName="GeneralTable" ref="B3:K10" totalsRowShown="0">
-  <autoFilter ref="B3:K10" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}" name="GeneralTable" displayName="GeneralTable" ref="B3:O11" totalsRowShown="0">
+  <autoFilter ref="B3:O11" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}"/>
+  <tableColumns count="14">
     <tableColumn id="9" xr3:uid="{930AA11C-DBAD-449C-9AAB-58413DD653FF}" name="Reference-No."/>
     <tableColumn id="1" xr3:uid="{4EB90E3D-8138-420D-9685-23ED5E0CD304}" name="Post-No"/>
     <tableColumn id="2" xr3:uid="{92C57538-460C-4E03-9CB9-83B07236AA32}" name="CPU"/>
@@ -6057,9 +6344,13 @@
       <calculatedColumnFormula>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC9686E4-85C0-47F0-8897-2265DDE0051D}" name="PES ST"/>
+    <tableColumn id="6" xr3:uid="{374DB514-59D1-4DD5-9B7D-7CBBDA45F154}" name="Consumption ST"/>
+    <tableColumn id="13" xr3:uid="{10E1BD7B-CAF9-42F5-8914-D1310D8226D9}" name="Duration ST"/>
+    <tableColumn id="14" xr3:uid="{24DAABC1-44C6-41F4-932F-8FE2CC1373D1}" name="Average Power ST"/>
     <tableColumn id="5" xr3:uid="{12E62267-0D7D-4CE4-BBC7-A7856D373EEC}" name="PES MT"/>
-    <tableColumn id="6" xr3:uid="{374DB514-59D1-4DD5-9B7D-7CBBDA45F154}" name="Consumption ST"/>
     <tableColumn id="7" xr3:uid="{601EDF6E-3CF8-4495-BCA8-F12B64C740B5}" name="Consumption MT"/>
+    <tableColumn id="15" xr3:uid="{CE683E5F-B131-497D-9152-9159DF956534}" name="Duration MT"/>
+    <tableColumn id="16" xr3:uid="{27A65197-EB92-4DD2-BC96-E7065F4BE0F9}" name="Average Power MT"/>
     <tableColumn id="8" xr3:uid="{7CD33795-D9C5-445A-86EB-6454E2C11F57}" name="BB-Code" dataDxfId="0">
       <calculatedColumnFormula>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</calculatedColumnFormula>
     </tableColumn>
@@ -6331,10 +6622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K10"/>
+  <dimension ref="B2:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6342,22 +6633,26 @@
     <col min="1" max="1" width="5.5546875" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -6375,19 +6670,31 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -6408,20 +6715,20 @@
         <v>133.62</v>
       </c>
       <c r="H4">
+        <v>10168</v>
+      </c>
+      <c r="K4">
         <v>2586.7600000000002</v>
       </c>
-      <c r="I4">
-        <v>10168</v>
-      </c>
-      <c r="J4">
+      <c r="L4">
         <v>2649</v>
       </c>
-      <c r="K4" t="str">
+      <c r="O4" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
         <v>1|AMD Ryzen 7 4700U (Renoir)|CrazyIvan|3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -6442,20 +6749,20 @@
         <v>45.76</v>
       </c>
       <c r="H5">
+        <v>32112</v>
+      </c>
+      <c r="K5">
         <v>1386.39</v>
       </c>
-      <c r="I5">
-        <v>32112</v>
-      </c>
-      <c r="J5">
+      <c r="L5">
         <v>7223</v>
       </c>
-      <c r="K5" t="str">
+      <c r="O5" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
         <v>2|AMD Ryzen 5 3600 (Matisse)|Lyka|6</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -6476,153 +6783,199 @@
         <v>127.76</v>
       </c>
       <c r="H6">
+        <v>9839</v>
+      </c>
+      <c r="K6">
         <v>885.22</v>
       </c>
-      <c r="I6">
-        <v>9839</v>
-      </c>
-      <c r="J6">
+      <c r="L6">
         <v>3912</v>
       </c>
-      <c r="K6" t="str">
+      <c r="O6" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
         <v>3|Intel i7 1065G (IceLake)|Naitsabes|7</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="str">
+        <v>25</v>
+      </c>
+      <c r="F7" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
-        <v>Ryzen 7 4750G (Renoir) [4]</v>
+        <v>AMD Razyen 9 5950X (Vermeer) [4]</v>
       </c>
       <c r="G7">
-        <v>153.88</v>
+        <v>55.41</v>
       </c>
       <c r="H7">
-        <v>2637.56</v>
+        <v>35920</v>
       </c>
       <c r="I7">
-        <v>10352</v>
+        <v>502.43</v>
       </c>
       <c r="J7">
-        <v>5262</v>
-      </c>
-      <c r="K7" t="str">
+        <v>71.489999999999995</v>
+      </c>
+      <c r="K7">
+        <v>4779.3</v>
+      </c>
+      <c r="L7">
+        <v>6242</v>
+      </c>
+      <c r="M7">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="N7">
+        <v>186.22</v>
+      </c>
+      <c r="O7" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>4|Ryzen 7 4750G (Renoir)|Poekel|18</v>
+        <v>4|AMD Razyen 9 5950X (Vermeer)|dosenfisch24|14</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
-        <v>AMD Razyen 7 3700X (Matisse) [5]</v>
+        <v>AMDRyzen 7 4750G (Renoir) [5]</v>
       </c>
       <c r="G8">
-        <v>51.8</v>
+        <v>153.88</v>
       </c>
       <c r="H8">
-        <v>2058.48</v>
-      </c>
-      <c r="I8">
-        <v>30057</v>
-      </c>
-      <c r="J8">
-        <v>6377</v>
-      </c>
-      <c r="K8" s="1" t="str">
+        <v>10352</v>
+      </c>
+      <c r="K8">
+        <v>2637.56</v>
+      </c>
+      <c r="L8">
+        <v>5262</v>
+      </c>
+      <c r="O8" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>5|AMD Razyen 7 3700X (Matisse)|Tigershark|27</v>
+        <v>5|AMDRyzen 7 4750G (Renoir)|Poekel|18</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
-        <v>AMD Ryzen 7 4750U [6]</v>
+        <v>AMD Razyen 7 3700X (Matisse) [6]</v>
       </c>
       <c r="G9">
-        <v>137.88</v>
+        <v>51.8</v>
       </c>
       <c r="H9">
-        <v>3599.63</v>
-      </c>
-      <c r="I9">
-        <v>10396</v>
-      </c>
-      <c r="J9">
-        <v>2029</v>
-      </c>
-      <c r="K9" s="1" t="str">
+        <v>30057</v>
+      </c>
+      <c r="K9">
+        <v>2058.48</v>
+      </c>
+      <c r="L9">
+        <v>6377</v>
+      </c>
+      <c r="O9" s="1" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>6|AMD Ryzen 7 4750U|dosenfisch24|29</v>
+        <v>6|AMD Razyen 7 3700X (Matisse)|Tigershark|27</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
       <c r="C10">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
-        <v>??? [7]</v>
+        <v>AMD Ryzen 7 4750U (Renoir) [7]</v>
       </c>
       <c r="G10">
+        <v>137.88</v>
+      </c>
+      <c r="H10">
+        <v>10396</v>
+      </c>
+      <c r="K10">
+        <v>3599.63</v>
+      </c>
+      <c r="L10">
+        <v>2029</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>7|AMD Ryzen 7 4750U (Renoir)|dosenfisch24|29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
+        <v>??? [8]</v>
+      </c>
+      <c r="G11">
         <v>52.94</v>
       </c>
-      <c r="H10">
+      <c r="H11">
+        <v>37274</v>
+      </c>
+      <c r="K11">
         <v>5760.71</v>
       </c>
-      <c r="I10">
-        <v>37274</v>
-      </c>
-      <c r="J10">
+      <c r="L11">
         <v>4507</v>
       </c>
-      <c r="K10" s="1" t="str">
+      <c r="O11" s="1" t="str">
         <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>7|???|Sweepi|32</v>
+        <v>8|???|Sweepi|32</v>
       </c>
     </row>
   </sheetData>
@@ -6636,16 +6989,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6F6CD-AB6C-41CA-A4F9-5492FC969623}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
@@ -6660,7 +7013,7 @@
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4">
         <v>45.76</v>
@@ -6668,7 +7021,7 @@
     </row>
     <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4">
         <v>51.8</v>
@@ -6676,7 +7029,7 @@
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4">
         <v>52.94</v>
@@ -6684,42 +7037,50 @@
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4">
-        <v>127.76</v>
+        <v>55.41</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4">
-        <v>133.62</v>
+        <v>127.76</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4">
-        <v>137.88</v>
+        <v>133.62</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4">
-        <v>153.88</v>
+        <v>137.88</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4">
+        <v>153.88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4">
-        <v>703.63999999999987</v>
+      <c r="C11" s="4">
+        <v>759.05</v>
       </c>
     </row>
   </sheetData>
@@ -6730,7 +7091,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2B96D4-491E-48C1-A9CD-50F5C88BFD81}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
@@ -6739,7 +7100,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
@@ -6749,12 +7110,12 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5">
         <v>37274</v>
@@ -6762,58 +7123,66 @@
     </row>
     <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5">
-        <v>32112</v>
+        <v>35920</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5">
-        <v>30057</v>
+        <v>32112</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5">
-        <v>10396</v>
+        <v>30057</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5">
-        <v>10352</v>
+        <v>10396</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5">
-        <v>10168</v>
+        <v>10352</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5">
-        <v>9839</v>
+        <v>10168</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5">
+        <v>9839</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
-        <v>140198</v>
+      <c r="C11" s="5">
+        <v>176118</v>
       </c>
     </row>
   </sheetData>
@@ -6824,7 +7193,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94310CC2-D69A-4FCA-BA74-8F5DF32F63B3}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
@@ -6833,7 +7202,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
@@ -6843,12 +7212,12 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4">
         <v>885.22</v>
@@ -6856,7 +7225,7 @@
     </row>
     <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4">
         <v>1386.39</v>
@@ -6864,7 +7233,7 @@
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4">
         <v>2058.48</v>
@@ -6872,7 +7241,7 @@
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4">
         <v>2586.7600000000002</v>
@@ -6880,7 +7249,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4">
         <v>2637.56</v>
@@ -6888,7 +7257,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4">
         <v>3599.63</v>
@@ -6896,18 +7265,26 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4">
-        <v>5760.71</v>
+        <v>4779.3</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5760.71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4">
-        <v>18914.75</v>
+      <c r="C11" s="4">
+        <v>23694.050000000003</v>
       </c>
     </row>
   </sheetData>
@@ -6919,16 +7296,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1E4BCF-0D99-422A-A715-C65F85CECA2F}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
@@ -6938,71 +7315,79 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1">
         <v>7223</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1">
         <v>6377</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="4">
-        <v>5262</v>
+        <v>34</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6242</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4">
-        <v>4507</v>
+        <v>42</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5262</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4">
-        <v>3912</v>
+      <c r="C7" s="1">
+        <v>4507</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2649</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3912</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2029</v>
+        <v>30</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2649</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4">
-        <v>31959</v>
+      <c r="C11" s="1">
+        <v>38201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- excluded CB23 from suite - NEW Settings.txt for Path to CB23 installation - WIP optimize Power Package tracking - Debug garbage - minor visuals in ranking and Results
</commit_message>
<xml_diff>
--- a/Rankings.xlsx
+++ b/Rankings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\BrsVgl\PerformanceEfficiencySuite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742B216-7335-4487-8BB1-BE53E5EA3D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D5671-8A20-40E1-87FA-9DB9F2498373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResultsEntry" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId6"/>
-    <pivotCache cacheId="8" r:id="rId7"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>CPU</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Sweepi</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>AMD Ryzen 5 3600 (Matisse) [2]</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
   </si>
   <si>
     <t>AMD Razyen 7 3700X (Matisse) [6]</t>
-  </si>
-  <si>
-    <t>??? [8]</t>
   </si>
   <si>
     <t>AMD Razyen 9 5950X (Vermeer) [4]</t>
@@ -171,6 +165,51 @@
   </si>
   <si>
     <t>AMDRyzen 7 4750G (Renoir) [5]</t>
+  </si>
+  <si>
+    <t>Bemerkung</t>
+  </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>Energy saving mode</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 5900HS (Cezanne)</t>
+  </si>
+  <si>
+    <t>Battery / Better efficiency / HP: recommended</t>
+  </si>
+  <si>
+    <t>Intel Core i5-8365U (WHL)</t>
+  </si>
+  <si>
+    <t>MD_Enigma</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 5 PRO 4650G (Renoir)</t>
+  </si>
+  <si>
+    <t>25W</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 5 PRO 4650G (Renoir) [12]</t>
+  </si>
+  <si>
+    <t>Intel Core i5-8365U (WHL) [11]</t>
+  </si>
+  <si>
+    <t>AMD Razyen 9 5950X (Vermeer) [8]</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 5900HS (Cezanne) [10]</t>
+  </si>
+  <si>
+    <t>AMDRyzen 7 4750G (Renoir) [13]</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9 5900HS (Cezanne) [9]</t>
   </si>
 </sst>
 </file>
@@ -206,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -215,13 +254,19 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -514,7 +559,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="bg1"/>
                   </a:solidFill>
@@ -586,7 +631,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -628,9 +673,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PES ST'!$B$3:$B$11</c:f>
+              <c:f>'PES ST'!$B$3:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
@@ -638,32 +683,47 @@
                   <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>??? [8]</c:v>
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [8]</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>Intel Core i5-8365U (WHL) [11]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [9]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AMD Ryzen 5 PRO 4650G (Renoir) [12]</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [10]</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AMDRyzen 7 4750G (Renoir) [13]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PES ST'!$C$3:$C$11</c:f>
+              <c:f>'PES ST'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>45.76</c:v>
                 </c:pt>
@@ -677,16 +737,31 @@
                   <c:v>55.41</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>88.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>117.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>127.76</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>133.62</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>137.88</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>153.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>165.09</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>173.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,7 +780,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="80"/>
         <c:axId val="2136136704"/>
         <c:axId val="2136137120"/>
       </c:barChart>
@@ -738,7 +813,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -920,7 +995,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CB23 | Single-Thread | Consumption [J/Ws]</a:t>
+              <a:t>CB23 | Single-Thread | Consumption [J</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> or </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ws]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1268,7 +1351,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="bg1"/>
                   </a:solidFill>
@@ -1340,7 +1423,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -1382,11 +1465,11 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Consumption ST'!$B$3:$B$11</c:f>
+              <c:f>'Consumption ST'!$B$3:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>??? [8]</c:v>
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [8]</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
@@ -1398,26 +1481,41 @@
                   <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AMD Ryzen 5 PRO 4650G (Renoir) [12]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Intel Core i5-8365U (WHL) [11]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [10]</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>AMDRyzen 7 4750G (Renoir) [13]</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [9]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Consumption ST'!$C$3:$C$11</c:f>
+              <c:f>'Consumption ST'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>37274</c:v>
                 </c:pt>
@@ -1431,16 +1529,31 @@
                   <c:v>30057</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>12968</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11657</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10936</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>10396</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>10352</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>10168</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>9839</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9122</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1459,7 +1572,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="80"/>
         <c:axId val="2136136704"/>
         <c:axId val="2136137120"/>
       </c:barChart>
@@ -1492,7 +1605,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2022,7 +2135,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="bg1"/>
                   </a:solidFill>
@@ -2094,7 +2207,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -2136,64 +2249,94 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PES MT'!$B$3:$B$11</c:f>
+              <c:f>'PES MT'!$B$3:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Intel Core i5-8365U (WHL) [11]</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>AMD Ryzen 5 PRO 4650G (Renoir) [12]</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [10]</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [9]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>AMDRyzen 7 4750G (Renoir) [13]</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>??? [8]</c:v>
+                <c:pt idx="12">
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [8]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PES MT'!$C$3:$C$11</c:f>
+              <c:f>'PES MT'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>656.66</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>885.22</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1386.39</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>1464.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2058.48</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>2586.7600000000002</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>2637.56</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>3481.64</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3599.63</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
+                  <c:v>3815.05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4670.05</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4779.3</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>5760.71</c:v>
                 </c:pt>
               </c:numCache>
@@ -2213,7 +2356,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="80"/>
         <c:axId val="2136136704"/>
         <c:axId val="2136137120"/>
       </c:barChart>
@@ -2246,7 +2389,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2434,7 +2577,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Consumption [J/Ws]</a:t>
+              <a:t>Consumption [J or Ws]</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2951,7 +3094,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="bg1"/>
                   </a:solidFill>
@@ -3023,7 +3166,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -3065,65 +3208,95 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Consumption MT'!$B$3:$B$11</c:f>
+              <c:f>'Consumption MT'!$B$3:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>AMD Ryzen 5 3600 (Matisse) [2]</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>AMD Ryzen 5 PRO 4650G (Renoir) [12]</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>AMD Razyen 7 3700X (Matisse) [6]</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>AMD Razyen 9 5950X (Vermeer) [4]</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>AMDRyzen 7 4750G (Renoir) [5]</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>??? [8]</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>Intel Core i5-8365U (WHL) [11]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AMD Razyen 9 5950X (Vermeer) [8]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [10]</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Intel i7 1065G (IceLake) [3]</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>AMD Ryzen 7 4700U (Renoir) [1]</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>AMDRyzen 7 4750G (Renoir) [13]</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>AMD Ryzen 7 4750U (Renoir) [7]</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>AMD Ryzen 9 5900HS (Cezanne) [9]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Consumption MT'!$C$3:$C$11</c:f>
+              <c:f>'Consumption MT'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>7223</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6591</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6377</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6242</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5262</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>4575</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4507</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>4085</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3912</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>2649</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>2227</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3142,7 +3315,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="80"/>
         <c:axId val="2136136704"/>
         <c:axId val="2136137120"/>
       </c:barChart>
@@ -3175,7 +3348,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5502,8 +5675,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5539,14 +5712,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>120</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5582,14 +5755,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>120</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5625,14 +5798,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>120</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>335280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5663,13 +5836,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44370.982344444441" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{1C48AB18-201F-498F-BA2B-FB5C4F62805E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44371.851023495372" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="13" xr:uid="{77F125F5-FAEA-41C0-B4FE-830A225910E6}">
   <cacheSource type="worksheet">
-    <worksheetSource name="GeneralTable[[GraphLabel]:[PES MT]]"/>
+    <worksheetSource name="GeneralTable[[GraphLabel]:[Average Power MT]]"/>
   </cacheSource>
-  <cacheFields count="6">
+  <cacheFields count="9">
     <cacheField name="GraphLabel" numFmtId="0">
-      <sharedItems count="18">
+      <sharedItems count="14">
         <s v="AMD Ryzen 7 4700U (Renoir) [1]"/>
         <s v="AMD Ryzen 5 3600 (Matisse) [2]"/>
         <s v="Intel i7 1065G (IceLake) [3]"/>
@@ -5677,33 +5850,38 @@
         <s v="AMDRyzen 7 4750G (Renoir) [5]"/>
         <s v="AMD Razyen 7 3700X (Matisse) [6]"/>
         <s v="AMD Ryzen 7 4750U (Renoir) [7]"/>
-        <s v="??? [8]"/>
-        <s v="Ryzen 7 4750G (Renoir) [18]" u="1"/>
-        <s v="AMD Ryzen 7 4750U [6]" u="1"/>
-        <s v="Intel i7 1065G (IceLake) [7]" u="1"/>
-        <s v="AMD Ryzen 5 3600 (Matisse) [6]" u="1"/>
-        <s v="AMD Ryzen 7 4750U [7]" u="1"/>
-        <s v="??? [7]" u="1"/>
-        <s v="Ryzen 7 4750G (Renoir) [4]" u="1"/>
-        <s v="Ryzen 7 4750G (Renoir) [5]" u="1"/>
-        <s v="AMD Razyen 7 3700X (Matisse) [5]" u="1"/>
-        <s v="AMD Ryzen 7 4700U (Renoir) [3]" u="1"/>
+        <s v="AMD Razyen 9 5950X (Vermeer) [8]"/>
+        <s v="AMD Ryzen 9 5900HS (Cezanne) [9]"/>
+        <s v="AMD Ryzen 9 5900HS (Cezanne) [10]"/>
+        <s v="Intel Core i5-8365U (WHL) [11]"/>
+        <s v="AMD Ryzen 5 PRO 4650G (Renoir) [12]"/>
+        <s v="AMDRyzen 7 4750G (Renoir) [13]"/>
+        <s v="??? [8]" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="PES ST" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.76" maxValue="153.88"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.76" maxValue="173.7"/>
     </cacheField>
     <cacheField name="Consumption ST" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9839" maxValue="37274"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="6239" maxValue="37274"/>
     </cacheField>
     <cacheField name="Duration ST" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="502.43" maxValue="502.43"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="502.43" maxValue="1433.91"/>
     </cacheField>
     <cacheField name="Average Power ST" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="71.489999999999995" maxValue="71.489999999999995"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4.3499999999999996" maxValue="71.489999999999995"/>
     </cacheField>
     <cacheField name="PES MT" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="885.22" maxValue="5760.71"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="656.66" maxValue="5760.71"/>
+    </cacheField>
+    <cacheField name="Consumption MT" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1738" maxValue="7223"/>
+    </cacheField>
+    <cacheField name="Duration MT" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="33.520000000000003" maxValue="332.85"/>
+    </cacheField>
+    <cacheField name="Average Power MT" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="11.52" maxValue="186.22"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -5715,13 +5893,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44370.984763657405" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{77F125F5-FAEA-41C0-B4FE-830A225910E6}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Boris Vogel" refreshedDate="44371.851023958334" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="13" xr:uid="{1C48AB18-201F-498F-BA2B-FB5C4F62805E}">
   <cacheSource type="worksheet">
-    <worksheetSource name="GeneralTable[[GraphLabel]:[Average Power MT]]"/>
+    <worksheetSource name="GeneralTable[[GraphLabel]:[PES MT]]"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="6">
     <cacheField name="GraphLabel" numFmtId="0">
-      <sharedItems count="8">
+      <sharedItems count="24">
         <s v="AMD Ryzen 7 4700U (Renoir) [1]"/>
         <s v="AMD Ryzen 5 3600 (Matisse) [2]"/>
         <s v="Intel i7 1065G (IceLake) [3]"/>
@@ -5729,32 +5907,39 @@
         <s v="AMDRyzen 7 4750G (Renoir) [5]"/>
         <s v="AMD Razyen 7 3700X (Matisse) [6]"/>
         <s v="AMD Ryzen 7 4750U (Renoir) [7]"/>
-        <s v="??? [8]"/>
+        <s v="AMD Razyen 9 5950X (Vermeer) [8]"/>
+        <s v="AMD Ryzen 9 5900HS (Cezanne) [9]"/>
+        <s v="AMD Ryzen 9 5900HS (Cezanne) [10]"/>
+        <s v="Intel Core i5-8365U (WHL) [11]"/>
+        <s v="AMD Ryzen 5 PRO 4650G (Renoir) [12]"/>
+        <s v="AMDRyzen 7 4750G (Renoir) [13]"/>
+        <s v="Ryzen 7 4750G (Renoir) [18]" u="1"/>
+        <s v="AMD Ryzen 7 4750U [6]" u="1"/>
+        <s v="Intel i7 1065G (IceLake) [7]" u="1"/>
+        <s v="AMD Ryzen 5 3600 (Matisse) [6]" u="1"/>
+        <s v="AMD Ryzen 7 4750U [7]" u="1"/>
+        <s v="??? [7]" u="1"/>
+        <s v="??? [8]" u="1"/>
+        <s v="Ryzen 7 4750G (Renoir) [4]" u="1"/>
+        <s v="Ryzen 7 4750G (Renoir) [5]" u="1"/>
+        <s v="AMD Razyen 7 3700X (Matisse) [5]" u="1"/>
+        <s v="AMD Ryzen 7 4700U (Renoir) [3]" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="PES ST" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.76" maxValue="153.88"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="45.76" maxValue="173.7"/>
     </cacheField>
     <cacheField name="Consumption ST" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9839" maxValue="37274"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="6239" maxValue="37274"/>
     </cacheField>
     <cacheField name="Duration ST" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="502.43" maxValue="502.43"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="502.43" maxValue="1433.91"/>
     </cacheField>
     <cacheField name="Average Power ST" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="71.489999999999995" maxValue="71.489999999999995"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4.3499999999999996" maxValue="71.489999999999995"/>
     </cacheField>
     <cacheField name="PES MT" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="885.22" maxValue="5760.71"/>
-    </cacheField>
-    <cacheField name="Consumption MT" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2029" maxValue="7223"/>
-    </cacheField>
-    <cacheField name="Duration MT" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="33.520000000000003" maxValue="33.520000000000003"/>
-    </cacheField>
-    <cacheField name="Average Power MT" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="186.22" maxValue="186.22"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="656.66" maxValue="5760.71"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -5766,76 +5951,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
-  <r>
-    <x v="0"/>
-    <n v="133.62"/>
-    <n v="10168"/>
-    <m/>
-    <m/>
-    <n v="2586.7600000000002"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="45.76"/>
-    <n v="32112"/>
-    <m/>
-    <m/>
-    <n v="1386.39"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="127.76"/>
-    <n v="9839"/>
-    <m/>
-    <m/>
-    <n v="885.22"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="55.41"/>
-    <n v="35920"/>
-    <n v="502.43"/>
-    <n v="71.489999999999995"/>
-    <n v="4779.3"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="153.88"/>
-    <n v="10352"/>
-    <m/>
-    <m/>
-    <n v="2637.56"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="51.8"/>
-    <n v="30057"/>
-    <m/>
-    <m/>
-    <n v="2058.48"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="137.88"/>
-    <n v="10396"/>
-    <m/>
-    <m/>
-    <n v="3599.63"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="52.94"/>
-    <n v="37274"/>
-    <m/>
-    <m/>
-    <n v="5760.71"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="13">
   <r>
     <x v="0"/>
     <n v="133.62"/>
@@ -5924,33 +6040,203 @@
     <m/>
     <m/>
   </r>
+  <r>
+    <x v="8"/>
+    <n v="111.79"/>
+    <n v="6239"/>
+    <n v="1433.91"/>
+    <n v="4.3499999999999996"/>
+    <n v="3815.05"/>
+    <n v="1738"/>
+    <n v="150.85"/>
+    <n v="11.52"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="165.09"/>
+    <n v="10936"/>
+    <n v="553.86"/>
+    <n v="19.75"/>
+    <n v="3481.64"/>
+    <n v="4085"/>
+    <n v="70.3"/>
+    <n v="58.11"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="88.24"/>
+    <n v="11657"/>
+    <n v="972.15"/>
+    <n v="11.99"/>
+    <n v="656.66"/>
+    <n v="4575"/>
+    <n v="332.85"/>
+    <n v="13.75"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="117.42"/>
+    <n v="12968"/>
+    <n v="656.73"/>
+    <n v="19.75"/>
+    <n v="1464.99"/>
+    <n v="6591"/>
+    <n v="103.56"/>
+    <n v="63.65"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="173.7"/>
+    <n v="9122"/>
+    <n v="631.12"/>
+    <n v="14.45"/>
+    <n v="4670.05"/>
+    <n v="2227"/>
+    <n v="96.17"/>
+    <n v="23.15"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="13">
+  <r>
+    <x v="0"/>
+    <n v="133.62"/>
+    <n v="10168"/>
+    <m/>
+    <m/>
+    <n v="2586.7600000000002"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="45.76"/>
+    <n v="32112"/>
+    <m/>
+    <m/>
+    <n v="1386.39"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="127.76"/>
+    <n v="9839"/>
+    <m/>
+    <m/>
+    <n v="885.22"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="55.41"/>
+    <n v="35920"/>
+    <n v="502.43"/>
+    <n v="71.489999999999995"/>
+    <n v="4779.3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="153.88"/>
+    <n v="10352"/>
+    <m/>
+    <m/>
+    <n v="2637.56"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="51.8"/>
+    <n v="30057"/>
+    <m/>
+    <m/>
+    <n v="2058.48"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="137.88"/>
+    <n v="10396"/>
+    <m/>
+    <m/>
+    <n v="3599.63"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="52.94"/>
+    <n v="37274"/>
+    <m/>
+    <m/>
+    <n v="5760.71"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="111.79"/>
+    <n v="6239"/>
+    <n v="1433.91"/>
+    <n v="4.3499999999999996"/>
+    <n v="3815.05"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="165.09"/>
+    <n v="10936"/>
+    <n v="553.86"/>
+    <n v="19.75"/>
+    <n v="3481.64"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="88.24"/>
+    <n v="11657"/>
+    <n v="972.15"/>
+    <n v="11.99"/>
+    <n v="656.66"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="117.42"/>
+    <n v="12968"/>
+    <n v="656.73"/>
+    <n v="19.75"/>
+    <n v="1464.99"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="173.7"/>
+    <n v="9122"/>
+    <n v="631.12"/>
+    <n v="14.45"/>
+    <n v="4670.05"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53C9821C-4AAD-4B7A-89BF-B6F792D64CD3}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
-  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53C9821C-4AAD-4B7A-89BF-B6F792D64CD3}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+  <location ref="B2:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="19">
-        <item m="1" x="11"/>
-        <item m="1" x="17"/>
-        <item m="1" x="10"/>
-        <item m="1" x="8"/>
+      <items count="25">
+        <item m="1" x="16"/>
+        <item m="1" x="23"/>
+        <item m="1" x="15"/>
+        <item m="1" x="13"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="20"/>
+        <item m="1" x="22"/>
         <item m="1" x="14"/>
-        <item m="1" x="16"/>
-        <item m="1" x="9"/>
-        <item m="1" x="13"/>
+        <item m="1" x="18"/>
         <item x="3"/>
-        <item m="1" x="15"/>
+        <item m="1" x="21"/>
         <item x="5"/>
-        <item m="1" x="12"/>
-        <item x="7"/>
+        <item m="1" x="17"/>
+        <item m="1" x="19"/>
         <item x="4"/>
         <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -5972,7 +6258,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="14">
     <i>
       <x v="5"/>
     </i>
@@ -5980,10 +6266,19 @@
       <x v="13"/>
     </i>
     <i>
-      <x v="15"/>
+      <x v="18"/>
     </i>
     <i>
       <x v="11"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="22"/>
     </i>
     <i>
       <x v="6"/>
@@ -5996,6 +6291,12 @@
     </i>
     <i>
       <x v="16"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="23"/>
     </i>
     <i t="grand">
       <x/>
@@ -6031,29 +6332,35 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42BB440A-B501-4946-B14C-754D93D31B67}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42BB440A-B501-4946-B14C-754D93D31B67}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="B2:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="19">
-        <item m="1" x="11"/>
-        <item m="1" x="17"/>
-        <item m="1" x="10"/>
-        <item m="1" x="8"/>
+      <items count="25">
+        <item m="1" x="16"/>
+        <item m="1" x="23"/>
+        <item m="1" x="15"/>
+        <item m="1" x="13"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="20"/>
+        <item m="1" x="22"/>
         <item m="1" x="14"/>
-        <item m="1" x="16"/>
-        <item m="1" x="9"/>
-        <item m="1" x="13"/>
+        <item m="1" x="18"/>
         <item x="3"/>
-        <item m="1" x="15"/>
+        <item m="1" x="21"/>
         <item x="5"/>
-        <item m="1" x="12"/>
-        <item x="7"/>
+        <item m="1" x="17"/>
+        <item m="1" x="19"/>
         <item x="4"/>
         <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -6075,9 +6382,9 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="14">
     <i>
-      <x v="15"/>
+      <x v="18"/>
     </i>
     <i>
       <x v="11"/>
@@ -6087,6 +6394,15 @@
     </i>
     <i>
       <x v="13"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="20"/>
     </i>
     <i>
       <x v="17"/>
@@ -6099,6 +6415,12 @@
     </i>
     <i>
       <x v="6"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="19"/>
     </i>
     <i t="grand">
       <x/>
@@ -6134,29 +6456,35 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BEB41E7C-5AB2-4580-B381-A37610DCF2EB}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BEB41E7C-5AB2-4580-B381-A37610DCF2EB}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="B2:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="19">
-        <item m="1" x="11"/>
-        <item m="1" x="17"/>
-        <item m="1" x="10"/>
-        <item m="1" x="8"/>
+      <items count="25">
+        <item m="1" x="16"/>
+        <item m="1" x="23"/>
+        <item m="1" x="15"/>
+        <item m="1" x="13"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item m="1" x="20"/>
+        <item m="1" x="22"/>
         <item m="1" x="14"/>
-        <item m="1" x="16"/>
-        <item m="1" x="9"/>
-        <item m="1" x="13"/>
+        <item m="1" x="18"/>
         <item x="3"/>
-        <item m="1" x="15"/>
+        <item m="1" x="21"/>
         <item x="5"/>
-        <item m="1" x="12"/>
-        <item x="7"/>
+        <item m="1" x="17"/>
+        <item m="1" x="19"/>
         <item x="4"/>
         <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -6178,12 +6506,18 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="14">
+    <i>
+      <x v="21"/>
+    </i>
     <i>
       <x v="6"/>
     </i>
     <i>
       <x v="5"/>
+    </i>
+    <i>
+      <x v="22"/>
     </i>
     <i>
       <x v="13"/>
@@ -6195,13 +6529,22 @@
       <x v="16"/>
     </i>
     <i>
+      <x v="20"/>
+    </i>
+    <i>
       <x v="17"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="23"/>
     </i>
     <i>
       <x v="11"/>
     </i>
     <i>
-      <x v="15"/>
+      <x v="18"/>
     </i>
     <i t="grand">
       <x/>
@@ -6237,19 +6580,25 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2EE254DA-8EFF-4861-8DBF-B2F3ACC4A6C4}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="B2:C11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2EE254DA-8EFF-4861-8DBF-B2F3ACC4A6C4}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="B2:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="9">
+      <items count="15">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="5"/>
-        <item x="7"/>
+        <item m="1" x="13"/>
         <item x="4"/>
         <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -6274,9 +6623,12 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="14">
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="12"/>
     </i>
     <i>
       <x v="4"/>
@@ -6288,7 +6640,13 @@
       <x v="6"/>
     </i>
     <i>
-      <x v="5"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i>
       <x v="2"/>
@@ -6297,7 +6655,13 @@
       <x/>
     </i>
     <i>
+      <x v="13"/>
+    </i>
+    <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
     </i>
     <i t="grand">
       <x/>
@@ -6333,14 +6697,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}" name="GeneralTable" displayName="GeneralTable" ref="B3:O11" totalsRowShown="0">
-  <autoFilter ref="B3:O11" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}" name="GeneralTable" displayName="GeneralTable" ref="B3:P16" totalsRowShown="0">
+  <autoFilter ref="B3:P16" xr:uid="{D71527BF-35EF-41E4-9E51-2CB3A9570C24}"/>
+  <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{930AA11C-DBAD-449C-9AAB-58413DD653FF}" name="Reference-No."/>
     <tableColumn id="1" xr3:uid="{4EB90E3D-8138-420D-9685-23ED5E0CD304}" name="Post-No"/>
     <tableColumn id="2" xr3:uid="{92C57538-460C-4E03-9CB9-83B07236AA32}" name="CPU"/>
     <tableColumn id="3" xr3:uid="{F26113B1-1044-4D8E-AAF2-786269A14A78}" name="User"/>
-    <tableColumn id="10" xr3:uid="{17D81176-3AE4-44FC-9069-C773914DD128}" name="GraphLabel" dataDxfId="1">
+    <tableColumn id="11" xr3:uid="{C9A1EC67-185F-4C31-82BF-1FD4E60EEEB8}" name="Bemerkung" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{17D81176-3AE4-44FC-9069-C773914DD128}" name="GraphLabel" dataDxfId="2">
       <calculatedColumnFormula>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DC9686E4-85C0-47F0-8897-2265DDE0051D}" name="PES ST"/>
@@ -6352,7 +6717,7 @@
     <tableColumn id="15" xr3:uid="{CE683E5F-B131-497D-9152-9159DF956534}" name="Duration MT"/>
     <tableColumn id="16" xr3:uid="{27A65197-EB92-4DD2-BC96-E7065F4BE0F9}" name="Average Power MT"/>
     <tableColumn id="8" xr3:uid="{7CD33795-D9C5-445A-86EB-6454E2C11F57}" name="BB-Code" dataDxfId="0">
-      <calculatedColumnFormula>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</calculatedColumnFormula>
+      <calculatedColumnFormula>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6622,10 +6987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O11"/>
+  <dimension ref="B3:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6633,24 +6998,25 @@
     <col min="1" max="1" width="5.5546875" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="76.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -6664,37 +7030,40 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" t="s">
+      <c r="O3" t="s">
         <v>36</v>
       </c>
-      <c r="K3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -6707,28 +7076,31 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>AMD Ryzen 7 4700U (Renoir) [1]</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>133.62</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>10168</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2586.7600000000002</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>2649</v>
       </c>
-      <c r="O4" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>1|AMD Ryzen 7 4700U (Renoir)|CrazyIvan|3</v>
+      <c r="P4" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>1|AMD Ryzen 7 4700U (Renoir)|CrazyIvan|Battery / Better efficiency / HP: recommended|3</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -6741,28 +7113,29 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5" s="6"/>
+      <c r="G5" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>AMD Ryzen 5 3600 (Matisse) [2]</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>45.76</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>32112</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1386.39</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>7223</v>
       </c>
-      <c r="O5" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>2|AMD Ryzen 5 3600 (Matisse)|Lyka|6</v>
+      <c r="P5" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>2|AMD Ryzen 5 3600 (Matisse)|Lyka||6</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -6775,28 +7148,29 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" s="6"/>
+      <c r="G6" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>Intel i7 1065G (IceLake) [3]</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>127.76</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>9839</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>885.22</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>3912</v>
       </c>
-      <c r="O6" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>3|Intel i7 1065G (IceLake)|Naitsabes|7</v>
+      <c r="P6" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>3|Intel i7 1065G (IceLake)|Naitsabes||7</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -6804,45 +7178,46 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="6"/>
+      <c r="G7" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>AMD Razyen 9 5950X (Vermeer) [4]</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>55.41</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>35920</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>502.43</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>71.489999999999995</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>4779.3</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>6242</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>33.520000000000003</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>186.22</v>
       </c>
-      <c r="O7" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>4|AMD Razyen 9 5950X (Vermeer)|dosenfisch24|14</v>
+      <c r="P7" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>4|AMD Razyen 9 5950X (Vermeer)|dosenfisch24||14</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -6850,33 +7225,34 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="str">
+      <c r="F8" s="6"/>
+      <c r="G8" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>AMDRyzen 7 4750G (Renoir) [5]</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>153.88</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>10352</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2637.56</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>5262</v>
       </c>
-      <c r="O8" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>5|AMDRyzen 7 4750G (Renoir)|Poekel|18</v>
+      <c r="P8" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>5|AMDRyzen 7 4750G (Renoir)|Poekel||18</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -6889,28 +7265,29 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="str">
+      <c r="F9" s="6"/>
+      <c r="G9" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>AMD Razyen 7 3700X (Matisse) [6]</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>51.8</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>30057</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>2058.48</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>6377</v>
       </c>
-      <c r="O9" s="1" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>6|AMD Razyen 7 3700X (Matisse)|Tigershark|27</v>
+      <c r="P9" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>6|AMD Razyen 7 3700X (Matisse)|Tigershark||27</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -6918,33 +7295,34 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1" t="str">
+      <c r="F10" s="6"/>
+      <c r="G10" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
         <v>AMD Ryzen 7 4750U (Renoir) [7]</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>137.88</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>10396</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>3599.63</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>2029</v>
       </c>
-      <c r="O10" s="1" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>7|AMD Ryzen 7 4750U (Renoir)|dosenfisch24|29</v>
+      <c r="P10" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>7|AMD Ryzen 7 4750U (Renoir)|dosenfisch24||29</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -6952,30 +7330,270 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="1" t="str">
+      <c r="F11" s="6"/>
+      <c r="G11" s="1" t="str">
         <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
-        <v>??? [8]</v>
-      </c>
-      <c r="G11">
+        <v>AMD Razyen 9 5950X (Vermeer) [8]</v>
+      </c>
+      <c r="H11">
         <v>52.94</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>37274</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>5760.71</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>4507</v>
       </c>
-      <c r="O11" s="1" t="str">
-        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
-        <v>8|???|Sweepi|32</v>
+      <c r="P11" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>8|AMD Razyen 9 5950X (Vermeer)|Sweepi||32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
+        <v>AMD Ryzen 9 5900HS (Cezanne) [9]</v>
+      </c>
+      <c r="H12">
+        <v>111.79</v>
+      </c>
+      <c r="I12">
+        <v>6239</v>
+      </c>
+      <c r="J12">
+        <v>1433.91</v>
+      </c>
+      <c r="K12">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="L12">
+        <v>3815.05</v>
+      </c>
+      <c r="M12">
+        <v>1738</v>
+      </c>
+      <c r="N12">
+        <v>150.85</v>
+      </c>
+      <c r="O12">
+        <v>11.52</v>
+      </c>
+      <c r="P12" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>9|AMD Ryzen 9 5900HS (Cezanne)|Monkey|Energy saving mode|42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1" t="str">
+        <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
+        <v>AMD Ryzen 9 5900HS (Cezanne) [10]</v>
+      </c>
+      <c r="H13">
+        <v>165.09</v>
+      </c>
+      <c r="I13">
+        <v>10936</v>
+      </c>
+      <c r="J13">
+        <v>553.86</v>
+      </c>
+      <c r="K13">
+        <v>19.75</v>
+      </c>
+      <c r="L13">
+        <v>3481.64</v>
+      </c>
+      <c r="M13">
+        <v>4085</v>
+      </c>
+      <c r="N13">
+        <v>70.3</v>
+      </c>
+      <c r="O13">
+        <v>58.11</v>
+      </c>
+      <c r="P13" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>10|AMD Ryzen 9 5900HS (Cezanne)|Monkey||44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1" t="str">
+        <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
+        <v>Intel Core i5-8365U (WHL) [11]</v>
+      </c>
+      <c r="H14">
+        <v>88.24</v>
+      </c>
+      <c r="I14">
+        <v>11657</v>
+      </c>
+      <c r="J14">
+        <v>972.15</v>
+      </c>
+      <c r="K14">
+        <v>11.99</v>
+      </c>
+      <c r="L14">
+        <v>656.66</v>
+      </c>
+      <c r="M14">
+        <v>4575</v>
+      </c>
+      <c r="N14">
+        <v>332.85</v>
+      </c>
+      <c r="O14">
+        <v>13.75</v>
+      </c>
+      <c r="P14" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>11|Intel Core i5-8365U (WHL)|MD_Enigma||54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1" t="str">
+        <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
+        <v>AMD Ryzen 5 PRO 4650G (Renoir) [12]</v>
+      </c>
+      <c r="H15">
+        <v>117.42</v>
+      </c>
+      <c r="I15">
+        <v>12968</v>
+      </c>
+      <c r="J15">
+        <v>656.73</v>
+      </c>
+      <c r="K15">
+        <v>19.75</v>
+      </c>
+      <c r="L15">
+        <v>1464.99</v>
+      </c>
+      <c r="M15">
+        <v>6591</v>
+      </c>
+      <c r="N15">
+        <v>103.56</v>
+      </c>
+      <c r="O15">
+        <v>63.65</v>
+      </c>
+      <c r="P15" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>12|AMD Ryzen 5 PRO 4650G (Renoir)|Tigershark||60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f>GeneralTable[[#This Row],[CPU]] &amp; " [" &amp;GeneralTable[[#This Row],[Reference-No.]] &amp; "]"</f>
+        <v>AMDRyzen 7 4750G (Renoir) [13]</v>
+      </c>
+      <c r="H16">
+        <v>173.7</v>
+      </c>
+      <c r="I16">
+        <v>9122</v>
+      </c>
+      <c r="J16">
+        <v>631.12</v>
+      </c>
+      <c r="K16">
+        <v>14.45</v>
+      </c>
+      <c r="L16">
+        <v>4670.05</v>
+      </c>
+      <c r="M16">
+        <v>2227</v>
+      </c>
+      <c r="N16">
+        <v>96.17</v>
+      </c>
+      <c r="O16">
+        <v>23.15</v>
+      </c>
+      <c r="P16" s="1" t="str">
+        <f>GeneralTable[[#This Row],[Reference-No.]]&amp;"|"&amp;GeneralTable[[#This Row],[CPU]]&amp;"|"&amp;GeneralTable[[#This Row],[User]]&amp;"|"&amp;GeneralTable[[#This Row],[Bemerkung]]&amp;"|"&amp;GeneralTable[[#This Row],[Post-No]]</f>
+        <v>13|AMDRyzen 7 4750G (Renoir)|Poekel|25W|47</v>
       </c>
     </row>
   </sheetData>
@@ -6989,21 +7607,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6F6CD-AB6C-41CA-A4F9-5492FC969623}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -7011,76 +7629,116 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4">
         <v>45.76</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4">
         <v>51.8</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4">
         <v>52.94</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4">
         <v>55.41</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="4">
+        <v>88.24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4">
+        <v>111.79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4">
+        <v>117.42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4">
+        <v>127.76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4">
-        <v>127.76</v>
+      <c r="C11" s="4">
+        <v>133.62</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4">
-        <v>133.62</v>
+    <row r="12" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="4">
+        <v>137.88</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="4">
-        <v>137.88</v>
+    <row r="13" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="4">
+        <v>153.88</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="4">
-        <v>153.88</v>
+    <row r="14" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="4">
+        <v>165.09</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="15" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4">
+        <v>173.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4">
-        <v>759.05</v>
+      <c r="C16" s="4">
+        <v>1415.29</v>
       </c>
     </row>
   </sheetData>
@@ -7091,21 +7749,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2B96D4-491E-48C1-A9CD-50F5C88BFD81}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -7113,76 +7771,116 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5">
         <v>37274</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5">
         <v>35920</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5">
         <v>32112</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5">
         <v>30057</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5">
+        <v>12968</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5">
+        <v>11657</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="5">
+        <v>10936</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5">
         <v>10396</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="5">
+    <row r="11" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="5">
         <v>10352</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5">
+    <row r="12" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5">
         <v>10168</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5">
+    <row r="13" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5">
         <v>9839</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="14" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5">
+        <v>9122</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5">
+        <v>6239</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5">
-        <v>176118</v>
+      <c r="C16" s="5">
+        <v>227040</v>
       </c>
     </row>
   </sheetData>
@@ -7193,21 +7891,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94310CC2-D69A-4FCA-BA74-8F5DF32F63B3}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -7215,76 +7913,116 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4">
-        <v>885.22</v>
+        <v>656.66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="4">
+        <v>885.22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4">
         <v>1386.39</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1464.99</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2058.48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2586.7600000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2637.56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3481.64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3599.63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3815.05</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4670.05</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4">
-        <v>2058.48</v>
+      <c r="C14" s="4">
+        <v>4779.3</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2586.7600000000002</v>
+    <row r="15" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5760.71</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2637.56</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="4">
-        <v>3599.63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="4">
-        <v>4779.3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="4">
-        <v>5760.71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="16" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4">
-        <v>23694.050000000003</v>
+      <c r="C16" s="4">
+        <v>37782.44</v>
       </c>
     </row>
   </sheetData>
@@ -7296,21 +8034,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1E4BCF-0D99-422A-A715-C65F85CECA2F}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
@@ -7318,76 +8056,116 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
         <v>7223</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6591</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6377</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1">
-        <v>6377</v>
+      <c r="C6" s="1">
+        <v>6242</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6242</v>
+    <row r="7" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5262</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5262</v>
+    <row r="8" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4575</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1">
+    <row r="9" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1">
         <v>4507</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="10" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1">
-        <v>3912</v>
+      <c r="C12" s="1">
+        <v>2649</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2649</v>
+    <row r="13" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2227</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="1">
+    <row r="14" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1">
         <v>2029</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="15" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1">
-        <v>38201</v>
+      <c r="C16" s="1">
+        <v>57417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>